<commit_message>
adding web automation tutorials (in progress)
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/ws-01.data.xlsx
+++ b/artifact/data/ws-01.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64C0E4B-660D-794D-9591-AFE008C21512}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996CBB48-7BD4-0C4E-9906-F68DECCBB9BC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="20480" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-21160" windowWidth="38400" windowHeight="7040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -36,10 +36,15 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -49,12 +54,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>true</t>
-  </si>
-  <si>
-    <t>800</t>
   </si>
   <si>
     <t>,</t>
@@ -66,19 +68,10 @@
     <t>false</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>nexial.scope.fallbackToPrevious</t>
   </si>
   <si>
     <t>nexial.scope.iteration</t>
-  </si>
-  <si>
-    <t>nexial.delayBetweenStepsMs</t>
-  </si>
-  <si>
-    <t>nexial.pollWaitMs</t>
   </si>
   <si>
     <t>nexial.failFast</t>
@@ -216,7 +209,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="5">
     <dxf>
       <font>
         <b val="0"/>
@@ -279,71 +272,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -636,9 +564,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA10"/>
+  <dimension ref="A1:AAA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -651,7 +581,7 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1360,10 +1290,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -2069,10 +1999,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -2280,7 +2210,7 @@
       <c r="GX3"/>
       <c r="GY3"/>
       <c r="GZ3"/>
-      <c r="HA3" s="6"/>
+      <c r="HA3" s="4"/>
       <c r="HB3"/>
       <c r="HC3"/>
       <c r="HD3"/>
@@ -2774,11 +2704,11 @@
       <c r="ZX3"/>
       <c r="ZY3"/>
       <c r="ZZ3"/>
-      <c r="AAA3" s="6"/>
+      <c r="AAA3" s="5"/>
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -3487,10 +3417,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -4195,1453 +4125,35 @@
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="S6"/>
-      <c r="T6"/>
-      <c r="U6"/>
-      <c r="V6"/>
-      <c r="W6"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-      <c r="AB6"/>
-      <c r="AC6"/>
-      <c r="AD6"/>
-      <c r="AE6"/>
-      <c r="AF6"/>
-      <c r="AG6"/>
-      <c r="AH6"/>
-      <c r="AI6"/>
-      <c r="AJ6"/>
-      <c r="AK6"/>
-      <c r="AL6"/>
-      <c r="AM6"/>
-      <c r="AN6"/>
-      <c r="AO6"/>
-      <c r="AP6"/>
-      <c r="AQ6"/>
-      <c r="AR6"/>
-      <c r="AS6"/>
-      <c r="AT6"/>
-      <c r="AU6"/>
-      <c r="AV6"/>
-      <c r="AW6"/>
-      <c r="AX6"/>
-      <c r="AY6"/>
-      <c r="AZ6"/>
-      <c r="BA6"/>
-      <c r="BB6"/>
-      <c r="BC6"/>
-      <c r="BD6"/>
-      <c r="BE6"/>
-      <c r="BF6"/>
-      <c r="BG6"/>
-      <c r="BH6"/>
-      <c r="BI6"/>
-      <c r="BJ6"/>
-      <c r="BK6"/>
-      <c r="BL6"/>
-      <c r="BM6"/>
-      <c r="BN6"/>
-      <c r="BO6"/>
-      <c r="BP6"/>
-      <c r="BQ6"/>
-      <c r="BR6"/>
-      <c r="BS6"/>
-      <c r="BT6"/>
-      <c r="BU6"/>
-      <c r="BV6"/>
-      <c r="BW6"/>
-      <c r="BX6"/>
-      <c r="BY6"/>
-      <c r="BZ6"/>
-      <c r="CA6"/>
-      <c r="CB6"/>
-      <c r="CC6"/>
-      <c r="CD6"/>
-      <c r="CE6"/>
-      <c r="CF6"/>
-      <c r="CG6"/>
-      <c r="CH6"/>
-      <c r="CI6"/>
-      <c r="CJ6"/>
-      <c r="CK6"/>
-      <c r="CL6"/>
-      <c r="CM6"/>
-      <c r="CN6"/>
-      <c r="CO6"/>
-      <c r="CP6"/>
-      <c r="CQ6"/>
-      <c r="CR6"/>
-      <c r="CS6"/>
-      <c r="CT6"/>
-      <c r="CU6"/>
-      <c r="CV6"/>
-      <c r="CW6"/>
-      <c r="CX6"/>
-      <c r="CY6"/>
-      <c r="CZ6"/>
-      <c r="DA6"/>
-      <c r="DB6"/>
-      <c r="DC6"/>
-      <c r="DD6"/>
-      <c r="DE6"/>
-      <c r="DF6"/>
-      <c r="DG6"/>
-      <c r="DH6"/>
-      <c r="DI6"/>
-      <c r="DJ6"/>
-      <c r="DK6"/>
-      <c r="DL6"/>
-      <c r="DM6"/>
-      <c r="DN6"/>
-      <c r="DO6"/>
-      <c r="DP6"/>
-      <c r="DQ6"/>
-      <c r="DR6"/>
-      <c r="DS6"/>
-      <c r="DT6"/>
-      <c r="DU6"/>
-      <c r="DV6"/>
-      <c r="DW6"/>
-      <c r="DX6"/>
-      <c r="DY6"/>
-      <c r="DZ6"/>
-      <c r="EA6"/>
-      <c r="EB6"/>
-      <c r="EC6"/>
-      <c r="ED6"/>
-      <c r="EE6"/>
-      <c r="EF6"/>
-      <c r="EG6"/>
-      <c r="EH6"/>
-      <c r="EI6"/>
-      <c r="EJ6"/>
-      <c r="EK6"/>
-      <c r="EL6"/>
-      <c r="EM6"/>
-      <c r="EN6"/>
-      <c r="EO6"/>
-      <c r="EP6"/>
-      <c r="EQ6"/>
-      <c r="ER6"/>
-      <c r="ES6"/>
-      <c r="ET6"/>
-      <c r="EU6"/>
-      <c r="EV6"/>
-      <c r="EW6"/>
-      <c r="EX6"/>
-      <c r="EY6"/>
-      <c r="EZ6"/>
-      <c r="FA6"/>
-      <c r="FB6"/>
-      <c r="FC6"/>
-      <c r="FD6"/>
-      <c r="FE6"/>
-      <c r="FF6"/>
-      <c r="FG6"/>
-      <c r="FH6"/>
-      <c r="FI6"/>
-      <c r="FJ6"/>
-      <c r="FK6"/>
-      <c r="FL6"/>
-      <c r="FM6"/>
-      <c r="FN6"/>
-      <c r="FO6"/>
-      <c r="FP6"/>
-      <c r="FQ6"/>
-      <c r="FR6"/>
-      <c r="FS6"/>
-      <c r="FT6"/>
-      <c r="FU6"/>
-      <c r="FV6"/>
-      <c r="FW6"/>
-      <c r="FX6"/>
-      <c r="FY6"/>
-      <c r="FZ6"/>
-      <c r="GA6"/>
-      <c r="GB6"/>
-      <c r="GC6"/>
-      <c r="GD6"/>
-      <c r="GE6"/>
-      <c r="GF6"/>
-      <c r="GG6"/>
-      <c r="GH6"/>
-      <c r="GI6"/>
-      <c r="GJ6"/>
-      <c r="GK6"/>
-      <c r="GL6"/>
-      <c r="GM6"/>
-      <c r="GN6"/>
-      <c r="GO6"/>
-      <c r="GP6"/>
-      <c r="GQ6"/>
-      <c r="GR6"/>
-      <c r="GS6"/>
-      <c r="GT6"/>
-      <c r="GU6"/>
-      <c r="GV6"/>
-      <c r="GW6"/>
-      <c r="GX6"/>
-      <c r="GY6"/>
-      <c r="GZ6"/>
       <c r="HA6" s="4"/>
-      <c r="HB6"/>
-      <c r="HC6"/>
-      <c r="HD6"/>
-      <c r="HE6"/>
-      <c r="HF6"/>
-      <c r="HG6"/>
-      <c r="HH6"/>
-      <c r="HI6"/>
-      <c r="HJ6"/>
-      <c r="HK6"/>
-      <c r="HL6"/>
-      <c r="HM6"/>
-      <c r="HN6"/>
-      <c r="HO6"/>
-      <c r="HP6"/>
-      <c r="HQ6"/>
-      <c r="HR6"/>
-      <c r="HS6"/>
-      <c r="HT6"/>
-      <c r="HU6"/>
-      <c r="HV6"/>
-      <c r="HW6"/>
-      <c r="HX6"/>
-      <c r="HY6"/>
-      <c r="HZ6"/>
-      <c r="IA6"/>
-      <c r="IB6"/>
-      <c r="IC6"/>
-      <c r="ID6"/>
-      <c r="IE6"/>
-      <c r="IF6"/>
-      <c r="IG6"/>
-      <c r="IH6"/>
-      <c r="II6"/>
-      <c r="IJ6"/>
-      <c r="IK6"/>
-      <c r="IL6"/>
-      <c r="IM6"/>
-      <c r="IN6"/>
-      <c r="IO6"/>
-      <c r="IP6"/>
-      <c r="IQ6"/>
-      <c r="IR6"/>
-      <c r="IS6"/>
-      <c r="IT6"/>
-      <c r="IU6"/>
-      <c r="IV6"/>
-      <c r="IW6"/>
-      <c r="IX6"/>
-      <c r="IY6"/>
-      <c r="IZ6"/>
-      <c r="JA6"/>
-      <c r="JB6"/>
-      <c r="JC6"/>
-      <c r="JD6"/>
-      <c r="JE6"/>
-      <c r="JF6"/>
-      <c r="JG6"/>
-      <c r="JH6"/>
-      <c r="JI6"/>
-      <c r="JJ6"/>
-      <c r="JK6"/>
-      <c r="JL6"/>
-      <c r="JM6"/>
-      <c r="JN6"/>
-      <c r="JO6"/>
-      <c r="JP6"/>
-      <c r="JQ6"/>
-      <c r="JR6"/>
-      <c r="JS6"/>
-      <c r="JT6"/>
-      <c r="JU6"/>
-      <c r="JV6"/>
-      <c r="JW6"/>
-      <c r="JX6"/>
-      <c r="JY6"/>
-      <c r="JZ6"/>
-      <c r="KA6"/>
-      <c r="KB6"/>
-      <c r="KC6"/>
-      <c r="KD6"/>
-      <c r="KE6"/>
-      <c r="KF6"/>
-      <c r="KG6"/>
-      <c r="KH6"/>
-      <c r="KI6"/>
-      <c r="KJ6"/>
-      <c r="KK6"/>
-      <c r="KL6"/>
-      <c r="KM6"/>
-      <c r="KN6"/>
-      <c r="KO6"/>
-      <c r="KP6"/>
-      <c r="KQ6"/>
-      <c r="KR6"/>
-      <c r="KS6"/>
-      <c r="KT6"/>
-      <c r="KU6"/>
-      <c r="KV6"/>
-      <c r="KW6"/>
-      <c r="KX6"/>
-      <c r="KY6"/>
-      <c r="KZ6"/>
-      <c r="LA6"/>
-      <c r="LB6"/>
-      <c r="LC6"/>
-      <c r="LD6"/>
-      <c r="LE6"/>
-      <c r="LF6"/>
-      <c r="LG6"/>
-      <c r="LH6"/>
-      <c r="LI6"/>
-      <c r="LJ6"/>
-      <c r="LK6"/>
-      <c r="LL6"/>
-      <c r="LM6"/>
-      <c r="LN6"/>
-      <c r="LO6"/>
-      <c r="LP6"/>
-      <c r="LQ6"/>
-      <c r="LR6"/>
-      <c r="LS6"/>
-      <c r="LT6"/>
-      <c r="LU6"/>
-      <c r="LV6"/>
-      <c r="LW6"/>
-      <c r="LX6"/>
-      <c r="LY6"/>
-      <c r="LZ6"/>
-      <c r="MA6"/>
-      <c r="MB6"/>
-      <c r="MC6"/>
-      <c r="MD6"/>
-      <c r="ME6"/>
-      <c r="MF6"/>
-      <c r="MG6"/>
-      <c r="MH6"/>
-      <c r="MI6"/>
-      <c r="MJ6"/>
-      <c r="MK6"/>
-      <c r="ML6"/>
-      <c r="MM6"/>
-      <c r="MN6"/>
-      <c r="MO6"/>
-      <c r="MP6"/>
-      <c r="MQ6"/>
-      <c r="MR6"/>
-      <c r="MS6"/>
-      <c r="MT6"/>
-      <c r="MU6"/>
-      <c r="MV6"/>
-      <c r="MW6"/>
-      <c r="MX6"/>
-      <c r="MY6"/>
-      <c r="MZ6"/>
-      <c r="NA6"/>
-      <c r="NB6"/>
-      <c r="NC6"/>
-      <c r="ND6"/>
-      <c r="NE6"/>
-      <c r="NF6"/>
-      <c r="NG6"/>
-      <c r="NH6"/>
-      <c r="NI6"/>
-      <c r="NJ6"/>
-      <c r="NK6"/>
-      <c r="NL6"/>
-      <c r="NM6"/>
-      <c r="NN6"/>
-      <c r="NO6"/>
-      <c r="NP6"/>
-      <c r="NQ6"/>
-      <c r="NR6"/>
-      <c r="NS6"/>
-      <c r="NT6"/>
-      <c r="NU6"/>
-      <c r="NV6"/>
-      <c r="NW6"/>
-      <c r="NX6"/>
-      <c r="NY6"/>
-      <c r="NZ6"/>
-      <c r="OA6"/>
-      <c r="OB6"/>
-      <c r="OC6"/>
-      <c r="OD6"/>
-      <c r="OE6"/>
-      <c r="OF6"/>
-      <c r="OG6"/>
-      <c r="OH6"/>
-      <c r="OI6"/>
-      <c r="OJ6"/>
-      <c r="OK6"/>
-      <c r="OL6"/>
-      <c r="OM6"/>
-      <c r="ON6"/>
-      <c r="OO6"/>
-      <c r="OP6"/>
-      <c r="OQ6"/>
-      <c r="OR6"/>
-      <c r="OS6"/>
-      <c r="OT6"/>
-      <c r="OU6"/>
-      <c r="OV6"/>
-      <c r="OW6"/>
-      <c r="OX6"/>
-      <c r="OY6"/>
-      <c r="OZ6"/>
-      <c r="PA6"/>
-      <c r="PB6"/>
-      <c r="PC6"/>
-      <c r="PD6"/>
-      <c r="PE6"/>
-      <c r="PF6"/>
-      <c r="PG6"/>
-      <c r="PH6"/>
-      <c r="PI6"/>
-      <c r="PJ6"/>
-      <c r="PK6"/>
-      <c r="PL6"/>
-      <c r="PM6"/>
-      <c r="PN6"/>
-      <c r="PO6"/>
-      <c r="PP6"/>
-      <c r="PQ6"/>
-      <c r="PR6"/>
-      <c r="PS6"/>
-      <c r="PT6"/>
-      <c r="PU6"/>
-      <c r="PV6"/>
-      <c r="PW6"/>
-      <c r="PX6"/>
-      <c r="PY6"/>
-      <c r="PZ6"/>
-      <c r="QA6"/>
-      <c r="QB6"/>
-      <c r="QC6"/>
-      <c r="QD6"/>
-      <c r="QE6"/>
-      <c r="QF6"/>
-      <c r="QG6"/>
-      <c r="QH6"/>
-      <c r="QI6"/>
-      <c r="QJ6"/>
-      <c r="QK6"/>
-      <c r="QL6"/>
-      <c r="QM6"/>
-      <c r="QN6"/>
-      <c r="QO6"/>
-      <c r="QP6"/>
-      <c r="QQ6"/>
-      <c r="QR6"/>
-      <c r="QS6"/>
-      <c r="QT6"/>
-      <c r="QU6"/>
-      <c r="QV6"/>
-      <c r="QW6"/>
-      <c r="QX6"/>
-      <c r="QY6"/>
-      <c r="QZ6"/>
-      <c r="RA6"/>
-      <c r="RB6"/>
-      <c r="RC6"/>
-      <c r="RD6"/>
-      <c r="RE6"/>
-      <c r="RF6"/>
-      <c r="RG6"/>
-      <c r="RH6"/>
-      <c r="RI6"/>
-      <c r="RJ6"/>
-      <c r="RK6"/>
-      <c r="RL6"/>
-      <c r="RM6"/>
-      <c r="RN6"/>
-      <c r="RO6"/>
-      <c r="RP6"/>
-      <c r="RQ6"/>
-      <c r="RR6"/>
-      <c r="RS6"/>
-      <c r="RT6"/>
-      <c r="RU6"/>
-      <c r="RV6"/>
-      <c r="RW6"/>
-      <c r="RX6"/>
-      <c r="RY6"/>
-      <c r="RZ6"/>
-      <c r="SA6"/>
-      <c r="SB6"/>
-      <c r="SC6"/>
-      <c r="SD6"/>
-      <c r="SE6"/>
-      <c r="SF6"/>
-      <c r="SG6"/>
-      <c r="SH6"/>
-      <c r="SI6"/>
-      <c r="SJ6"/>
-      <c r="SK6"/>
-      <c r="SL6"/>
-      <c r="SM6"/>
-      <c r="SN6"/>
-      <c r="SO6"/>
-      <c r="SP6"/>
-      <c r="SQ6"/>
-      <c r="SR6"/>
-      <c r="SS6"/>
-      <c r="ST6"/>
-      <c r="SU6"/>
-      <c r="SV6"/>
-      <c r="SW6"/>
-      <c r="SX6"/>
-      <c r="SY6"/>
-      <c r="SZ6"/>
-      <c r="TA6"/>
-      <c r="TB6"/>
-      <c r="TC6"/>
-      <c r="TD6"/>
-      <c r="TE6"/>
-      <c r="TF6"/>
-      <c r="TG6"/>
-      <c r="TH6"/>
-      <c r="TI6"/>
-      <c r="TJ6"/>
-      <c r="TK6"/>
-      <c r="TL6"/>
-      <c r="TM6"/>
-      <c r="TN6"/>
-      <c r="TO6"/>
-      <c r="TP6"/>
-      <c r="TQ6"/>
-      <c r="TR6"/>
-      <c r="TS6"/>
-      <c r="TT6"/>
-      <c r="TU6"/>
-      <c r="TV6"/>
-      <c r="TW6"/>
-      <c r="TX6"/>
-      <c r="TY6"/>
-      <c r="TZ6"/>
-      <c r="UA6"/>
-      <c r="UB6"/>
-      <c r="UC6"/>
-      <c r="UD6"/>
-      <c r="UE6"/>
-      <c r="UF6"/>
-      <c r="UG6"/>
-      <c r="UH6"/>
-      <c r="UI6"/>
-      <c r="UJ6"/>
-      <c r="UK6"/>
-      <c r="UL6"/>
-      <c r="UM6"/>
-      <c r="UN6"/>
-      <c r="UO6"/>
-      <c r="UP6"/>
-      <c r="UQ6"/>
-      <c r="UR6"/>
-      <c r="US6"/>
-      <c r="UT6"/>
-      <c r="UU6"/>
-      <c r="UV6"/>
-      <c r="UW6"/>
-      <c r="UX6"/>
-      <c r="UY6"/>
-      <c r="UZ6"/>
-      <c r="VA6"/>
-      <c r="VB6"/>
-      <c r="VC6"/>
-      <c r="VD6"/>
-      <c r="VE6"/>
-      <c r="VF6"/>
-      <c r="VG6"/>
-      <c r="VH6"/>
-      <c r="VI6"/>
-      <c r="VJ6"/>
-      <c r="VK6"/>
-      <c r="VL6"/>
-      <c r="VM6"/>
-      <c r="VN6"/>
-      <c r="VO6"/>
-      <c r="VP6"/>
-      <c r="VQ6"/>
-      <c r="VR6"/>
-      <c r="VS6"/>
-      <c r="VT6"/>
-      <c r="VU6"/>
-      <c r="VV6"/>
-      <c r="VW6"/>
-      <c r="VX6"/>
-      <c r="VY6"/>
-      <c r="VZ6"/>
-      <c r="WA6"/>
-      <c r="WB6"/>
-      <c r="WC6"/>
-      <c r="WD6"/>
-      <c r="WE6"/>
-      <c r="WF6"/>
-      <c r="WG6"/>
-      <c r="WH6"/>
-      <c r="WI6"/>
-      <c r="WJ6"/>
-      <c r="WK6"/>
-      <c r="WL6"/>
-      <c r="WM6"/>
-      <c r="WN6"/>
-      <c r="WO6"/>
-      <c r="WP6"/>
-      <c r="WQ6"/>
-      <c r="WR6"/>
-      <c r="WS6"/>
-      <c r="WT6"/>
-      <c r="WU6"/>
-      <c r="WV6"/>
-      <c r="WW6"/>
-      <c r="WX6"/>
-      <c r="WY6"/>
-      <c r="WZ6"/>
-      <c r="XA6"/>
-      <c r="XB6"/>
-      <c r="XC6"/>
-      <c r="XD6"/>
-      <c r="XE6"/>
-      <c r="XF6"/>
-      <c r="XG6"/>
-      <c r="XH6"/>
-      <c r="XI6"/>
-      <c r="XJ6"/>
-      <c r="XK6"/>
-      <c r="XL6"/>
-      <c r="XM6"/>
-      <c r="XN6"/>
-      <c r="XO6"/>
-      <c r="XP6"/>
-      <c r="XQ6"/>
-      <c r="XR6"/>
-      <c r="XS6"/>
-      <c r="XT6"/>
-      <c r="XU6"/>
-      <c r="XV6"/>
-      <c r="XW6"/>
-      <c r="XX6"/>
-      <c r="XY6"/>
-      <c r="XZ6"/>
-      <c r="YA6"/>
-      <c r="YB6"/>
-      <c r="YC6"/>
-      <c r="YD6"/>
-      <c r="YE6"/>
-      <c r="YF6"/>
-      <c r="YG6"/>
-      <c r="YH6"/>
-      <c r="YI6"/>
-      <c r="YJ6"/>
-      <c r="YK6"/>
-      <c r="YL6"/>
-      <c r="YM6"/>
-      <c r="YN6"/>
-      <c r="YO6"/>
-      <c r="YP6"/>
-      <c r="YQ6"/>
-      <c r="YR6"/>
-      <c r="YS6"/>
-      <c r="YT6"/>
-      <c r="YU6"/>
-      <c r="YV6"/>
-      <c r="YW6"/>
-      <c r="YX6"/>
-      <c r="YY6"/>
-      <c r="YZ6"/>
-      <c r="ZA6"/>
-      <c r="ZB6"/>
-      <c r="ZC6"/>
-      <c r="ZD6"/>
-      <c r="ZE6"/>
-      <c r="ZF6"/>
-      <c r="ZG6"/>
-      <c r="ZH6"/>
-      <c r="ZI6"/>
-      <c r="ZJ6"/>
-      <c r="ZK6"/>
-      <c r="ZL6"/>
-      <c r="ZM6"/>
-      <c r="ZN6"/>
-      <c r="ZO6"/>
-      <c r="ZP6"/>
-      <c r="ZQ6"/>
-      <c r="ZR6"/>
-      <c r="ZS6"/>
-      <c r="ZT6"/>
-      <c r="ZU6"/>
-      <c r="ZV6"/>
-      <c r="ZW6"/>
-      <c r="ZX6"/>
-      <c r="ZY6"/>
-      <c r="ZZ6"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7"/>
-      <c r="V7"/>
-      <c r="W7"/>
-      <c r="X7"/>
-      <c r="Y7"/>
-      <c r="Z7"/>
-      <c r="AA7"/>
-      <c r="AB7"/>
-      <c r="AC7"/>
-      <c r="AD7"/>
-      <c r="AE7"/>
-      <c r="AF7"/>
-      <c r="AG7"/>
-      <c r="AH7"/>
-      <c r="AI7"/>
-      <c r="AJ7"/>
-      <c r="AK7"/>
-      <c r="AL7"/>
-      <c r="AM7"/>
-      <c r="AN7"/>
-      <c r="AO7"/>
-      <c r="AP7"/>
-      <c r="AQ7"/>
-      <c r="AR7"/>
-      <c r="AS7"/>
-      <c r="AT7"/>
-      <c r="AU7"/>
-      <c r="AV7"/>
-      <c r="AW7"/>
-      <c r="AX7"/>
-      <c r="AY7"/>
-      <c r="AZ7"/>
-      <c r="BA7"/>
-      <c r="BB7"/>
-      <c r="BC7"/>
-      <c r="BD7"/>
-      <c r="BE7"/>
-      <c r="BF7"/>
-      <c r="BG7"/>
-      <c r="BH7"/>
-      <c r="BI7"/>
-      <c r="BJ7"/>
-      <c r="BK7"/>
-      <c r="BL7"/>
-      <c r="BM7"/>
-      <c r="BN7"/>
-      <c r="BO7"/>
-      <c r="BP7"/>
-      <c r="BQ7"/>
-      <c r="BR7"/>
-      <c r="BS7"/>
-      <c r="BT7"/>
-      <c r="BU7"/>
-      <c r="BV7"/>
-      <c r="BW7"/>
-      <c r="BX7"/>
-      <c r="BY7"/>
-      <c r="BZ7"/>
-      <c r="CA7"/>
-      <c r="CB7"/>
-      <c r="CC7"/>
-      <c r="CD7"/>
-      <c r="CE7"/>
-      <c r="CF7"/>
-      <c r="CG7"/>
-      <c r="CH7"/>
-      <c r="CI7"/>
-      <c r="CJ7"/>
-      <c r="CK7"/>
-      <c r="CL7"/>
-      <c r="CM7"/>
-      <c r="CN7"/>
-      <c r="CO7"/>
-      <c r="CP7"/>
-      <c r="CQ7"/>
-      <c r="CR7"/>
-      <c r="CS7"/>
-      <c r="CT7"/>
-      <c r="CU7"/>
-      <c r="CV7"/>
-      <c r="CW7"/>
-      <c r="CX7"/>
-      <c r="CY7"/>
-      <c r="CZ7"/>
-      <c r="DA7"/>
-      <c r="DB7"/>
-      <c r="DC7"/>
-      <c r="DD7"/>
-      <c r="DE7"/>
-      <c r="DF7"/>
-      <c r="DG7"/>
-      <c r="DH7"/>
-      <c r="DI7"/>
-      <c r="DJ7"/>
-      <c r="DK7"/>
-      <c r="DL7"/>
-      <c r="DM7"/>
-      <c r="DN7"/>
-      <c r="DO7"/>
-      <c r="DP7"/>
-      <c r="DQ7"/>
-      <c r="DR7"/>
-      <c r="DS7"/>
-      <c r="DT7"/>
-      <c r="DU7"/>
-      <c r="DV7"/>
-      <c r="DW7"/>
-      <c r="DX7"/>
-      <c r="DY7"/>
-      <c r="DZ7"/>
-      <c r="EA7"/>
-      <c r="EB7"/>
-      <c r="EC7"/>
-      <c r="ED7"/>
-      <c r="EE7"/>
-      <c r="EF7"/>
-      <c r="EG7"/>
-      <c r="EH7"/>
-      <c r="EI7"/>
-      <c r="EJ7"/>
-      <c r="EK7"/>
-      <c r="EL7"/>
-      <c r="EM7"/>
-      <c r="EN7"/>
-      <c r="EO7"/>
-      <c r="EP7"/>
-      <c r="EQ7"/>
-      <c r="ER7"/>
-      <c r="ES7"/>
-      <c r="ET7"/>
-      <c r="EU7"/>
-      <c r="EV7"/>
-      <c r="EW7"/>
-      <c r="EX7"/>
-      <c r="EY7"/>
-      <c r="EZ7"/>
-      <c r="FA7"/>
-      <c r="FB7"/>
-      <c r="FC7"/>
-      <c r="FD7"/>
-      <c r="FE7"/>
-      <c r="FF7"/>
-      <c r="FG7"/>
-      <c r="FH7"/>
-      <c r="FI7"/>
-      <c r="FJ7"/>
-      <c r="FK7"/>
-      <c r="FL7"/>
-      <c r="FM7"/>
-      <c r="FN7"/>
-      <c r="FO7"/>
-      <c r="FP7"/>
-      <c r="FQ7"/>
-      <c r="FR7"/>
-      <c r="FS7"/>
-      <c r="FT7"/>
-      <c r="FU7"/>
-      <c r="FV7"/>
-      <c r="FW7"/>
-      <c r="FX7"/>
-      <c r="FY7"/>
-      <c r="FZ7"/>
-      <c r="GA7"/>
-      <c r="GB7"/>
-      <c r="GC7"/>
-      <c r="GD7"/>
-      <c r="GE7"/>
-      <c r="GF7"/>
-      <c r="GG7"/>
-      <c r="GH7"/>
-      <c r="GI7"/>
-      <c r="GJ7"/>
-      <c r="GK7"/>
-      <c r="GL7"/>
-      <c r="GM7"/>
-      <c r="GN7"/>
-      <c r="GO7"/>
-      <c r="GP7"/>
-      <c r="GQ7"/>
-      <c r="GR7"/>
-      <c r="GS7"/>
-      <c r="GT7"/>
-      <c r="GU7"/>
-      <c r="GV7"/>
-      <c r="GW7"/>
-      <c r="GX7"/>
-      <c r="GY7"/>
-      <c r="GZ7"/>
       <c r="HA7" s="4"/>
-      <c r="HB7"/>
-      <c r="HC7"/>
-      <c r="HD7"/>
-      <c r="HE7"/>
-      <c r="HF7"/>
-      <c r="HG7"/>
-      <c r="HH7"/>
-      <c r="HI7"/>
-      <c r="HJ7"/>
-      <c r="HK7"/>
-      <c r="HL7"/>
-      <c r="HM7"/>
-      <c r="HN7"/>
-      <c r="HO7"/>
-      <c r="HP7"/>
-      <c r="HQ7"/>
-      <c r="HR7"/>
-      <c r="HS7"/>
-      <c r="HT7"/>
-      <c r="HU7"/>
-      <c r="HV7"/>
-      <c r="HW7"/>
-      <c r="HX7"/>
-      <c r="HY7"/>
-      <c r="HZ7"/>
-      <c r="IA7"/>
-      <c r="IB7"/>
-      <c r="IC7"/>
-      <c r="ID7"/>
-      <c r="IE7"/>
-      <c r="IF7"/>
-      <c r="IG7"/>
-      <c r="IH7"/>
-      <c r="II7"/>
-      <c r="IJ7"/>
-      <c r="IK7"/>
-      <c r="IL7"/>
-      <c r="IM7"/>
-      <c r="IN7"/>
-      <c r="IO7"/>
-      <c r="IP7"/>
-      <c r="IQ7"/>
-      <c r="IR7"/>
-      <c r="IS7"/>
-      <c r="IT7"/>
-      <c r="IU7"/>
-      <c r="IV7"/>
-      <c r="IW7"/>
-      <c r="IX7"/>
-      <c r="IY7"/>
-      <c r="IZ7"/>
-      <c r="JA7"/>
-      <c r="JB7"/>
-      <c r="JC7"/>
-      <c r="JD7"/>
-      <c r="JE7"/>
-      <c r="JF7"/>
-      <c r="JG7"/>
-      <c r="JH7"/>
-      <c r="JI7"/>
-      <c r="JJ7"/>
-      <c r="JK7"/>
-      <c r="JL7"/>
-      <c r="JM7"/>
-      <c r="JN7"/>
-      <c r="JO7"/>
-      <c r="JP7"/>
-      <c r="JQ7"/>
-      <c r="JR7"/>
-      <c r="JS7"/>
-      <c r="JT7"/>
-      <c r="JU7"/>
-      <c r="JV7"/>
-      <c r="JW7"/>
-      <c r="JX7"/>
-      <c r="JY7"/>
-      <c r="JZ7"/>
-      <c r="KA7"/>
-      <c r="KB7"/>
-      <c r="KC7"/>
-      <c r="KD7"/>
-      <c r="KE7"/>
-      <c r="KF7"/>
-      <c r="KG7"/>
-      <c r="KH7"/>
-      <c r="KI7"/>
-      <c r="KJ7"/>
-      <c r="KK7"/>
-      <c r="KL7"/>
-      <c r="KM7"/>
-      <c r="KN7"/>
-      <c r="KO7"/>
-      <c r="KP7"/>
-      <c r="KQ7"/>
-      <c r="KR7"/>
-      <c r="KS7"/>
-      <c r="KT7"/>
-      <c r="KU7"/>
-      <c r="KV7"/>
-      <c r="KW7"/>
-      <c r="KX7"/>
-      <c r="KY7"/>
-      <c r="KZ7"/>
-      <c r="LA7"/>
-      <c r="LB7"/>
-      <c r="LC7"/>
-      <c r="LD7"/>
-      <c r="LE7"/>
-      <c r="LF7"/>
-      <c r="LG7"/>
-      <c r="LH7"/>
-      <c r="LI7"/>
-      <c r="LJ7"/>
-      <c r="LK7"/>
-      <c r="LL7"/>
-      <c r="LM7"/>
-      <c r="LN7"/>
-      <c r="LO7"/>
-      <c r="LP7"/>
-      <c r="LQ7"/>
-      <c r="LR7"/>
-      <c r="LS7"/>
-      <c r="LT7"/>
-      <c r="LU7"/>
-      <c r="LV7"/>
-      <c r="LW7"/>
-      <c r="LX7"/>
-      <c r="LY7"/>
-      <c r="LZ7"/>
-      <c r="MA7"/>
-      <c r="MB7"/>
-      <c r="MC7"/>
-      <c r="MD7"/>
-      <c r="ME7"/>
-      <c r="MF7"/>
-      <c r="MG7"/>
-      <c r="MH7"/>
-      <c r="MI7"/>
-      <c r="MJ7"/>
-      <c r="MK7"/>
-      <c r="ML7"/>
-      <c r="MM7"/>
-      <c r="MN7"/>
-      <c r="MO7"/>
-      <c r="MP7"/>
-      <c r="MQ7"/>
-      <c r="MR7"/>
-      <c r="MS7"/>
-      <c r="MT7"/>
-      <c r="MU7"/>
-      <c r="MV7"/>
-      <c r="MW7"/>
-      <c r="MX7"/>
-      <c r="MY7"/>
-      <c r="MZ7"/>
-      <c r="NA7"/>
-      <c r="NB7"/>
-      <c r="NC7"/>
-      <c r="ND7"/>
-      <c r="NE7"/>
-      <c r="NF7"/>
-      <c r="NG7"/>
-      <c r="NH7"/>
-      <c r="NI7"/>
-      <c r="NJ7"/>
-      <c r="NK7"/>
-      <c r="NL7"/>
-      <c r="NM7"/>
-      <c r="NN7"/>
-      <c r="NO7"/>
-      <c r="NP7"/>
-      <c r="NQ7"/>
-      <c r="NR7"/>
-      <c r="NS7"/>
-      <c r="NT7"/>
-      <c r="NU7"/>
-      <c r="NV7"/>
-      <c r="NW7"/>
-      <c r="NX7"/>
-      <c r="NY7"/>
-      <c r="NZ7"/>
-      <c r="OA7"/>
-      <c r="OB7"/>
-      <c r="OC7"/>
-      <c r="OD7"/>
-      <c r="OE7"/>
-      <c r="OF7"/>
-      <c r="OG7"/>
-      <c r="OH7"/>
-      <c r="OI7"/>
-      <c r="OJ7"/>
-      <c r="OK7"/>
-      <c r="OL7"/>
-      <c r="OM7"/>
-      <c r="ON7"/>
-      <c r="OO7"/>
-      <c r="OP7"/>
-      <c r="OQ7"/>
-      <c r="OR7"/>
-      <c r="OS7"/>
-      <c r="OT7"/>
-      <c r="OU7"/>
-      <c r="OV7"/>
-      <c r="OW7"/>
-      <c r="OX7"/>
-      <c r="OY7"/>
-      <c r="OZ7"/>
-      <c r="PA7"/>
-      <c r="PB7"/>
-      <c r="PC7"/>
-      <c r="PD7"/>
-      <c r="PE7"/>
-      <c r="PF7"/>
-      <c r="PG7"/>
-      <c r="PH7"/>
-      <c r="PI7"/>
-      <c r="PJ7"/>
-      <c r="PK7"/>
-      <c r="PL7"/>
-      <c r="PM7"/>
-      <c r="PN7"/>
-      <c r="PO7"/>
-      <c r="PP7"/>
-      <c r="PQ7"/>
-      <c r="PR7"/>
-      <c r="PS7"/>
-      <c r="PT7"/>
-      <c r="PU7"/>
-      <c r="PV7"/>
-      <c r="PW7"/>
-      <c r="PX7"/>
-      <c r="PY7"/>
-      <c r="PZ7"/>
-      <c r="QA7"/>
-      <c r="QB7"/>
-      <c r="QC7"/>
-      <c r="QD7"/>
-      <c r="QE7"/>
-      <c r="QF7"/>
-      <c r="QG7"/>
-      <c r="QH7"/>
-      <c r="QI7"/>
-      <c r="QJ7"/>
-      <c r="QK7"/>
-      <c r="QL7"/>
-      <c r="QM7"/>
-      <c r="QN7"/>
-      <c r="QO7"/>
-      <c r="QP7"/>
-      <c r="QQ7"/>
-      <c r="QR7"/>
-      <c r="QS7"/>
-      <c r="QT7"/>
-      <c r="QU7"/>
-      <c r="QV7"/>
-      <c r="QW7"/>
-      <c r="QX7"/>
-      <c r="QY7"/>
-      <c r="QZ7"/>
-      <c r="RA7"/>
-      <c r="RB7"/>
-      <c r="RC7"/>
-      <c r="RD7"/>
-      <c r="RE7"/>
-      <c r="RF7"/>
-      <c r="RG7"/>
-      <c r="RH7"/>
-      <c r="RI7"/>
-      <c r="RJ7"/>
-      <c r="RK7"/>
-      <c r="RL7"/>
-      <c r="RM7"/>
-      <c r="RN7"/>
-      <c r="RO7"/>
-      <c r="RP7"/>
-      <c r="RQ7"/>
-      <c r="RR7"/>
-      <c r="RS7"/>
-      <c r="RT7"/>
-      <c r="RU7"/>
-      <c r="RV7"/>
-      <c r="RW7"/>
-      <c r="RX7"/>
-      <c r="RY7"/>
-      <c r="RZ7"/>
-      <c r="SA7"/>
-      <c r="SB7"/>
-      <c r="SC7"/>
-      <c r="SD7"/>
-      <c r="SE7"/>
-      <c r="SF7"/>
-      <c r="SG7"/>
-      <c r="SH7"/>
-      <c r="SI7"/>
-      <c r="SJ7"/>
-      <c r="SK7"/>
-      <c r="SL7"/>
-      <c r="SM7"/>
-      <c r="SN7"/>
-      <c r="SO7"/>
-      <c r="SP7"/>
-      <c r="SQ7"/>
-      <c r="SR7"/>
-      <c r="SS7"/>
-      <c r="ST7"/>
-      <c r="SU7"/>
-      <c r="SV7"/>
-      <c r="SW7"/>
-      <c r="SX7"/>
-      <c r="SY7"/>
-      <c r="SZ7"/>
-      <c r="TA7"/>
-      <c r="TB7"/>
-      <c r="TC7"/>
-      <c r="TD7"/>
-      <c r="TE7"/>
-      <c r="TF7"/>
-      <c r="TG7"/>
-      <c r="TH7"/>
-      <c r="TI7"/>
-      <c r="TJ7"/>
-      <c r="TK7"/>
-      <c r="TL7"/>
-      <c r="TM7"/>
-      <c r="TN7"/>
-      <c r="TO7"/>
-      <c r="TP7"/>
-      <c r="TQ7"/>
-      <c r="TR7"/>
-      <c r="TS7"/>
-      <c r="TT7"/>
-      <c r="TU7"/>
-      <c r="TV7"/>
-      <c r="TW7"/>
-      <c r="TX7"/>
-      <c r="TY7"/>
-      <c r="TZ7"/>
-      <c r="UA7"/>
-      <c r="UB7"/>
-      <c r="UC7"/>
-      <c r="UD7"/>
-      <c r="UE7"/>
-      <c r="UF7"/>
-      <c r="UG7"/>
-      <c r="UH7"/>
-      <c r="UI7"/>
-      <c r="UJ7"/>
-      <c r="UK7"/>
-      <c r="UL7"/>
-      <c r="UM7"/>
-      <c r="UN7"/>
-      <c r="UO7"/>
-      <c r="UP7"/>
-      <c r="UQ7"/>
-      <c r="UR7"/>
-      <c r="US7"/>
-      <c r="UT7"/>
-      <c r="UU7"/>
-      <c r="UV7"/>
-      <c r="UW7"/>
-      <c r="UX7"/>
-      <c r="UY7"/>
-      <c r="UZ7"/>
-      <c r="VA7"/>
-      <c r="VB7"/>
-      <c r="VC7"/>
-      <c r="VD7"/>
-      <c r="VE7"/>
-      <c r="VF7"/>
-      <c r="VG7"/>
-      <c r="VH7"/>
-      <c r="VI7"/>
-      <c r="VJ7"/>
-      <c r="VK7"/>
-      <c r="VL7"/>
-      <c r="VM7"/>
-      <c r="VN7"/>
-      <c r="VO7"/>
-      <c r="VP7"/>
-      <c r="VQ7"/>
-      <c r="VR7"/>
-      <c r="VS7"/>
-      <c r="VT7"/>
-      <c r="VU7"/>
-      <c r="VV7"/>
-      <c r="VW7"/>
-      <c r="VX7"/>
-      <c r="VY7"/>
-      <c r="VZ7"/>
-      <c r="WA7"/>
-      <c r="WB7"/>
-      <c r="WC7"/>
-      <c r="WD7"/>
-      <c r="WE7"/>
-      <c r="WF7"/>
-      <c r="WG7"/>
-      <c r="WH7"/>
-      <c r="WI7"/>
-      <c r="WJ7"/>
-      <c r="WK7"/>
-      <c r="WL7"/>
-      <c r="WM7"/>
-      <c r="WN7"/>
-      <c r="WO7"/>
-      <c r="WP7"/>
-      <c r="WQ7"/>
-      <c r="WR7"/>
-      <c r="WS7"/>
-      <c r="WT7"/>
-      <c r="WU7"/>
-      <c r="WV7"/>
-      <c r="WW7"/>
-      <c r="WX7"/>
-      <c r="WY7"/>
-      <c r="WZ7"/>
-      <c r="XA7"/>
-      <c r="XB7"/>
-      <c r="XC7"/>
-      <c r="XD7"/>
-      <c r="XE7"/>
-      <c r="XF7"/>
-      <c r="XG7"/>
-      <c r="XH7"/>
-      <c r="XI7"/>
-      <c r="XJ7"/>
-      <c r="XK7"/>
-      <c r="XL7"/>
-      <c r="XM7"/>
-      <c r="XN7"/>
-      <c r="XO7"/>
-      <c r="XP7"/>
-      <c r="XQ7"/>
-      <c r="XR7"/>
-      <c r="XS7"/>
-      <c r="XT7"/>
-      <c r="XU7"/>
-      <c r="XV7"/>
-      <c r="XW7"/>
-      <c r="XX7"/>
-      <c r="XY7"/>
-      <c r="XZ7"/>
-      <c r="YA7"/>
-      <c r="YB7"/>
-      <c r="YC7"/>
-      <c r="YD7"/>
-      <c r="YE7"/>
-      <c r="YF7"/>
-      <c r="YG7"/>
-      <c r="YH7"/>
-      <c r="YI7"/>
-      <c r="YJ7"/>
-      <c r="YK7"/>
-      <c r="YL7"/>
-      <c r="YM7"/>
-      <c r="YN7"/>
-      <c r="YO7"/>
-      <c r="YP7"/>
-      <c r="YQ7"/>
-      <c r="YR7"/>
-      <c r="YS7"/>
-      <c r="YT7"/>
-      <c r="YU7"/>
-      <c r="YV7"/>
-      <c r="YW7"/>
-      <c r="YX7"/>
-      <c r="YY7"/>
-      <c r="YZ7"/>
-      <c r="ZA7"/>
-      <c r="ZB7"/>
-      <c r="ZC7"/>
-      <c r="ZD7"/>
-      <c r="ZE7"/>
-      <c r="ZF7"/>
-      <c r="ZG7"/>
-      <c r="ZH7"/>
-      <c r="ZI7"/>
-      <c r="ZJ7"/>
-      <c r="ZK7"/>
-      <c r="ZL7"/>
-      <c r="ZM7"/>
-      <c r="ZN7"/>
-      <c r="ZO7"/>
-      <c r="ZP7"/>
-      <c r="ZQ7"/>
-      <c r="ZR7"/>
-      <c r="ZS7"/>
-      <c r="ZT7"/>
-      <c r="ZU7"/>
-      <c r="ZV7"/>
-      <c r="ZW7"/>
-      <c r="ZX7"/>
-      <c r="ZY7"/>
-      <c r="ZZ7"/>
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703">
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
-    <row r="9" spans="1:703">
-      <c r="HA9" s="4"/>
-      <c r="AAA9" s="5"/>
-    </row>
-    <row r="10" spans="1:703">
-      <c r="HA10" s="4"/>
-      <c r="AAA10" s="5"/>
-    </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="6" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="5" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="9" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="7" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>